<commit_message>
UI and local sqlite3 database
</commit_message>
<xml_diff>
--- a/data/San Lorenzo.xlsx
+++ b/data/San Lorenzo.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,35 +553,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>41052285</t>
+          <t>ML82002263</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>19638 Hathaway Ave</t>
+          <t>17269 Via La Jolla</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hayward</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>94541</t>
+          <t>94580</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>797000</v>
+        <v>808000</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
         <v>2</v>
       </c>
       <c r="H2" t="n">
-        <v>1624</v>
+        <v>1431</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
@@ -592,89 +592,89 @@
       <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>No HOA fee</t>
-        </is>
+      <c r="L2" t="n">
+        <v>13</v>
       </c>
       <c r="M2" t="n">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/Hayward/19638-Hathaway-Ave-94541/home/856870</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/17269-Via-La-Jolla-94580/home/1876538</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Open House - 12:00 - 3:00 PM</t>
+          <t>Open House - 2:00 - 4:30 PM</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Mar 10, 12:00PM</t>
+          <t>Apr 13, 2:00PM</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>78413605</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0</v>
+        <v>113019204</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>Daniel Donate</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>Welcome to this charming 4-bedroom, 2-bathroom Hayward home boasting delightful updates and ample space. Step inside to discover a tastefully renovated interior, featuring a spacious layout perfect for comfortable living. The highlight of this residence is its expansive primary bedroom, providing a serene retreat for relaxation. Whether you're unwinding after a long day or enjoying the morning sunshine, this bedroom offers a peaceful sanctuary. Conveniently located near freeways, parks, shopping centers, and restaurants, this home ensures easy access to everyday amenities and entertainment options, making it an ideal choice for families and individuals alike. Experience the epitome of conve</t>
+          <t>Nestled in the charming San Lorenzo Village, this stunning home offers comfort and convenience. With three bedrooms and two bathrooms spread over 1431 sq/ft, this property boasts an open floor plan that invites natural light and warmth. This home has been thoughtfully expanded to include a spacious family room and direct access to the backyard, perfect for gatherings and relaxation. Close to schools, the post office, banks, and community parks, this home offers the best of suburban living in a fabulous neighborhood.</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>CHERRYLAND AREA</t>
+          <t>SAN LORENZO</t>
         </is>
       </c>
       <c r="V2" t="n">
-        <v>37.6757111</v>
+        <v>37.6683195</v>
       </c>
       <c r="W2" t="n">
-        <v>-122.1134619</v>
+        <v>-122.1358186</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>41052122</t>
+          <t>41091674</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15803 Via Nueva</t>
+          <t>20145 Royal Ave</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>San Lorenzo</t>
+          <t>Hayward</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>94580</t>
+          <t>94541</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>869950</v>
+        <v>1500000</v>
       </c>
       <c r="F3" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="H3" t="n">
-        <v>1181</v>
+        <v>3082</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -685,15 +685,17 @@
       <c r="K3" t="b">
         <v>0</v>
       </c>
-      <c r="L3" t="n">
-        <v>11</v>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>No HOA fee</t>
+        </is>
       </c>
       <c r="M3" t="n">
-        <v>1955</v>
+        <v>1972</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/15803-Via-Nueva-94580/home/1009983</t>
+          <t>https://www.redfin.com/CA/Hayward-Acres/20145-Royal-Ave-94541/home/1827236</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -707,42 +709,44 @@
         </is>
       </c>
       <c r="Q3" t="n">
-        <v>171290731</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0</v>
+        <v>128780800</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>Thomy Clements</t>
+          <t>David Weglarz</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>Welcome to your dream home nestled in the heart of The San Lorenzo Village! This charming single-family residence boasts 3 cozy bedrooms and 2 bathrooms, all w/ in a spacious 1,181 Sq/Ft of living space. Plank hardwood floors guide you through the light-filled rooms, creating an inviting atmosphere that you'll love coming home to. Situated on a desirable corner lot, this home offers a perfect blend of privacy and curb appeal. The NEW ROOF and NEW HEATER ensure that you'll enjoy years of worry-free comfort, while the property's bright and airy ambiance is perfect for entertaining or simply relaxing with loved ones. The garage offers ample storage  &amp;amp;  a sturdy workbench , perfect for tack</t>
+          <t>A rare triplex offering three distinct homes on one spacious ±0.43 acre parcel. Ideal for owner occupants looking to offset their mortgage with 2 currently occupied homes ($4,700/mo rent) or investors looking to capitalize on rental demand. Per public records, the total livable, building square footage is ±3,082; there's a sizeable garage that has ADU conversion potential. Located in un-incorporated Hayward, each home was built in varying generation. Front (4 bed/1.5 bath) home delivered vacant and ready for your finishing touches. Between I-880 to East and Hesperian Blvd to West, the location has easy access to Hwy 92 and 238. Close to schools, shopping and downtown BART.</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>SAN LORENZO VILG</t>
+          <t>Hayward</t>
         </is>
       </c>
       <c r="V3" t="n">
-        <v>37.6746004</v>
+        <v>37.6696704</v>
       </c>
       <c r="W3" t="n">
-        <v>-122.1475143</v>
+        <v>-122.1157407</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>41051512</t>
+          <t>41092927</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>920 Elgin St Unit G</t>
+          <t>1136 Via Esperanza</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -756,16 +760,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>450000</v>
+        <v>925000</v>
       </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
         <v>2</v>
       </c>
       <c r="H4" t="n">
-        <v>900</v>
+        <v>1615</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -777,65 +781,63 @@
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>400</v>
+        <v>13</v>
       </c>
       <c r="M4" t="n">
-        <v>1990</v>
+        <v>1950</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/920-Elgin-St-94580/unit-G/home/1810369</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/1136-Via-Esperanza-94580/home/943033</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Open House - 1:00 - 5:00 PM</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Apr 13, 1:00PM</t>
         </is>
       </c>
       <c r="Q4" t="n">
-        <v>753413814</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+        <v>180221858</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>Chin Fong</t>
+          <t>Ines Eiras</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>Cozy and affordable home conveniently located in a secure and gated complex on the quite street, near local freeways and walking distant to BART Station. This second level unit offers an open floor plan, laminate and carpet  flooring in the living space. The kitchen is high functional space with tile counters, and plenty of cabinet storage. A sliding glass door bring in lots of light. Patio gives extra space for home garden, relax area or an extra storage area. It also offers a laundry closet with hook-ups, two good size bathrooms, a walk-in closet off the master bedroom and two parking spaces, one of which is covered. This is a great opportunity for you to call it home!   OH 3/9  &amp;amp;  3/</t>
+          <t>Rare 4/2 one story Modern Move In Ready Updated Village 1615 sft Home features new floor coverings, designer colors, quartz countertops, quality wood details and moldings, ample open space, recessed lighting and brushed nickel fixtures, modern hardware, luxurious hall bath tub shower combination. Entertain in spacious bright family room, cozy patio area and enjoy the spacious backyard on 5610 sft lot with citrus trees. Conveniently located with easy access to major freeways, shopping, parks, schools, and San Mateo Bridge. San Lorenzo Village Homes Association HOA $150 annual dues.</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>ASHLAND</t>
+          <t>SAN LORENZO VILG</t>
         </is>
       </c>
       <c r="V4" t="n">
-        <v>37.6914613</v>
+        <v>37.6675061</v>
       </c>
       <c r="W4" t="n">
-        <v>-122.1164255</v>
+        <v>-122.1290231</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>41051040</t>
+          <t>ML82002057</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16147 Via Milos</t>
+          <t>2119 via barrett</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -849,7 +851,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>799000</v>
+        <v>845000</v>
       </c>
       <c r="F5" t="n">
         <v>3</v>
@@ -858,7 +860,7 @@
         <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>1231</v>
+        <v>1131</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -873,83 +875,85 @@
         <v>13</v>
       </c>
       <c r="M5" t="n">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/16147-Via-Milos-94580/home/1384592</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/2119-Via-Barrett-94580/home/928369</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Open House - 2:00 - 4:30 PM</t>
+          <t>Open House - 1:00 - 5:00 PM</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Mar 10, 2:00PM</t>
+          <t>Apr 13, 1:00PM</t>
         </is>
       </c>
       <c r="Q5" t="n">
-        <v>847381416</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
+        <v>187101857</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>Mayling Trinh</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t xml:space="preserve">This delightful detached home offers a serene escape while being conveniently close to schools, parks, shopping, and dining. Boasting 3 bedrooms and 2 full bathrooms, this well-maintained residence provides the perfect canvas for your dream living space. Upon entering, you're greeted by a warm and inviting atmosphere, accentuated by original hardwood floors and a skylight in the kitchen. The kitchen features newer appliances. Step outside to discover a covered patio area, enveloped by blooming flowers and mature fruit trees, including fig, lemon, and pepino melons. Whether you're entertaining guests or simply unwinding after a long day. Don't miss the opportunity to make this charming home </t>
+          <t xml:space="preserve">Charming San Lorenzo Village Home with ADU Potential ! Situated on a rare 7,200 sq. ft. corner lot with easy access, this beautifully maintained 3-bedroom, 2-bathroom home in San Lorenzo Village offers both comfort and investment potential. The open-concept kitchen and living area create a bright, inviting space perfect for modern living and entertaining. The kitchen is a chefs delight with spacious island, stainless steel appliances, and recessed lighting in the living room that brightens every corner. Additional highlights include a beautiful hardwood floor, new paint, new light fixtures in the bathroom and a two-car garage with a new garage door opener. Step outside to a spacious, fully </t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>SAN LORENZO VILG</t>
+          <t>SAN LORENZO</t>
         </is>
       </c>
       <c r="V5" t="n">
-        <v>37.6693866</v>
+        <v>37.6737438</v>
       </c>
       <c r="W5" t="n">
-        <v>-122.1457535</v>
+        <v>-122.1512317</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>41051051</t>
+          <t>41092648</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17263 Via La Jolla</t>
+          <t>19235 Times Ave</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>San Lorenzo</t>
+          <t>Hayward</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>94580</t>
+          <t>94541</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>849000</v>
+        <v>880000</v>
       </c>
       <c r="F6" t="n">
         <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H6" t="n">
-        <v>1415</v>
+        <v>1624</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
@@ -960,64 +964,66 @@
       <c r="K6" t="b">
         <v>0</v>
       </c>
-      <c r="L6" t="n">
-        <v>13</v>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>No HOA fee</t>
+        </is>
       </c>
       <c r="M6" t="n">
-        <v>1950</v>
+        <v>1952</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/17263-Via-La-Jolla-94580/home/932117</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/19235-Times-Ave-94541/home/1856870</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Open House - 2:00 - 5:00 PM</t>
+          <t>Open House - 1:00 - 4:00 PM</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Mar 10, 2:00PM</t>
+          <t>Apr 13, 1:00PM</t>
         </is>
       </c>
       <c r="Q6" t="n">
-        <v>1028428841</v>
+        <v>300400875</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>Stephen Ng</t>
+          <t>Kara Cox</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>Welcome to your dream home in the heart of the family-friendly community of San Lorenzo! This charming 3-bedroom, 2-bathroom, 3 living room detached residence is a haven of comfort and style. This modern home offers luxurious finishes and upgrades conveniently located at San Lorenzo Village. It features a wide range of upgrades including a remodeled kitchen with new cabinets and stainless-steel appliances; two renovated bathrooms; a renewed garage with new garage door; smart home devices interior and exterior; a new furnace was installed just over a year ago; new lightings were installed in all rooms, kitchen, and bathrooms. The large space in the backyard has potential for Accessory Dwelli</t>
+          <t>Come see this well maintained, move-in ready home with large open-plan and modern kitchen. This home has a full bathroom, plus a half bathroom converted to a full bathroom without permits, as well as two common areas, newer roof, lateral line and appliances. The landscaped backyard features decking, raised beds, mature shrubbery and an apricot tree. The two car garage has finished walls, insulation and access to the house. Located with easy access to 880, BART and 92, this property also benefits from its placement in the San Lorenzo school district. Hardwood floors, natural light, fresh paint, Green Certified - Don’t miss this the chance to make this exceptional property your next hom</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>SAN LORENZO VILG</t>
+          <t>HAYWARD</t>
         </is>
       </c>
       <c r="V6" t="n">
-        <v>37.6684847</v>
+        <v>37.6773836</v>
       </c>
       <c r="W6" t="n">
-        <v>-122.1358167</v>
+        <v>-122.1136818</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>96712</t>
+          <t>41088770</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15750 Via Sorrento</t>
+          <t>1238 Via Dolorosa</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -1031,16 +1037,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>799500</v>
+        <v>865000</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>1348</v>
+        <v>1239</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
@@ -1051,17 +1057,15 @@
       <c r="K7" t="b">
         <v>0</v>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>No HOA fee</t>
-        </is>
+      <c r="L7" t="n">
+        <v>13</v>
       </c>
       <c r="M7" t="n">
-        <v>1956</v>
+        <v>1950</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/15750-Via-Sorrento-94580/home/1263503</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/1238-Via-Dolorosa-94580/home/756808</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -1074,76 +1078,72 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="Q7" t="n">
+        <v>2116938332</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>Ted Chen</t>
+          <t>Vincent De Rouen</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Nestled on a quiet street in the highly sought-after San Lorenzo Village, this freshly painted 3-bedroom, 1-bathroom home offers 1,239 sq. ft. of thoughtfully designed living space. Featuring custom hardwood floors, recessed lighting and copper plumbing, this home exudes timeless charm with a modern touch. The kitchen boasts elegant granite countertops, while the cozy bonus room and a wood-burning fireplace w/ blower creates the perfect retreat. Step outside to a spacious backyard, ideal for gardening, entertaining, or simply relaxing. The property includes a 1-car garage with Tesla Charging Station, Upgraded Electricity Box, 2-car driveway, and additional street parking for convenience. Ne</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>San Lorenzo</t>
+          <t>SAN LORENZO VILG</t>
         </is>
       </c>
       <c r="V7" t="n">
-        <v>37.6742555</v>
+        <v>37.6659618</v>
       </c>
       <c r="W7" t="n">
-        <v>-122.1528329</v>
+        <v>-122.1301119</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>41046503</t>
+          <t>ML81997755</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21164 Garden Ave</t>
+          <t>15928 Mills Ave</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Hayward</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>94541</t>
+          <t>94580</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>1100000</v>
+        <v>750000</v>
       </c>
       <c r="F8" t="n">
         <v>3</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>1438</v>
+        <v>1059</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
@@ -1154,11 +1154,11 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>1938</v>
+        <v>1951</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/Hayward/21164-Garden-Ave-94541/home/1793809</t>
+          <t>https://www.redfin.com/CA/Ashland/15928-Mills-Ave-94580/home/529939</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1172,42 +1172,44 @@
         </is>
       </c>
       <c r="Q8" t="n">
-        <v>6178862180</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
+        <v>1391541626</v>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>Meng Wu Moser</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>Do not disturb the tenants. Correction, the lot is almost 18,000sf and the house right next door 21132 Garden Ave is also for sale. Flat level land. Great opportunity for developers or someone looks to build a family complex in this huge lot. Convenient location to shoppings and freeways. Centrally located in the SF Bay Area, minutes away to HW 92 to get to SF peninsula.</t>
+          <t>Last weekend. Come see while you get a chance! Welcome to this beautifully updated 3-bedroom, 1-bathroom home in the heart of San Lorenzo's Hesperian Garden neighborhood. Recently refreshed with new interior paint and modern flooring, this residence seamlessly blends contemporary style with classic charm. The open-concept kitchen invites culinary creativity and effortless entertaining, while the expansive backyard offers a private oasis for relaxation, gardening, or play. Notably, the property provides convenient RV parking, catering to travel enthusiasts. Positioned directly across from a serene park, and within walking distance to schools, public transportation, and shopping, this home en</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>HAYWARD</t>
+          <t>SAN LORENZO</t>
         </is>
       </c>
       <c r="V8" t="n">
-        <v>37.6689404</v>
+        <v>37.6931007</v>
       </c>
       <c r="W8" t="n">
-        <v>-122.1111926</v>
+        <v>-122.1230865</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>41048442</t>
+          <t>41090964</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>183 E Lewelling Blvd</t>
+          <t>1328 Via El Monte</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1221,16 +1223,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>1600000</v>
+        <v>869000</v>
       </c>
       <c r="F9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H9" t="n">
-        <v>2648</v>
+        <v>1425</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -1247,11 +1249,11 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>1920</v>
+        <v>1951</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/183-E-Lewelling-Blvd-94580/home/1847919</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/1328-Via-El-Monte-94580/home/953648</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1265,7 +1267,7 @@
         </is>
       </c>
       <c r="Q9" t="n">
-        <v>3849767951</v>
+        <v>1433909312</v>
       </c>
       <c r="R9" t="inlineStr">
         <is>
@@ -1274,35 +1276,35 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>Kathi Townsend</t>
+          <t>Tammi Hannah</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>ATTENTION DEVELOPERS! THIS PROPERTY BOASTS ENDLESS POSSIBILITIES. Two lots equaling 1 Acre. Check with County to see how many units can be built on property. Possible uses include a family compound or possibly multiple families, business use to park or store multiple vehicles, i. e. , Landscapers can have equipment and plants and family all on one property. You can build ADU's and have family and income. Main house has 2 bedrooms, 1 bath, bonus room, partial basement and is approximately 1500 sq. ft. Property also has 3 separate rental units. Each detached rental unit is approximately 300 sq. ft. is either a studio or has 1 bedroom, 1 bath and kitchenette. Property to be sold in conjunction</t>
+          <t>Open House Sat, 4/12, from Noon -3pm First time on the market! This home has been loved by the same family for 74 years! Located in the heart of the highly sought after San Lorenzo Village, Via El Monte offers 1425sf of living space situated on a 5671sf lot that includes a large shed and ample room for a potential ADU. This freshly painted home features 3 bedrooms, 2 full baths, wood floors, and a family room off the kitchen with new carpet and a skylight that maximizes the natural light. A new water heater was installed in February '25 in the large 2-car garage. Your new home is walking distance to Elementary, Middle and High Schools, centrally located near by restaurants, shopping, Del Re</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>ASHLAND</t>
+          <t>SAN LORENZO VILG</t>
         </is>
       </c>
       <c r="V9" t="n">
-        <v>37.6864823</v>
+        <v>37.673946</v>
       </c>
       <c r="W9" t="n">
-        <v>-122.1190638</v>
+        <v>-122.1367775</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>41048441</t>
+          <t>41089296</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>181 E Lewelling Blvd</t>
+          <t>934 Delano St</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1316,23 +1318,23 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1300000</v>
+        <v>749000</v>
       </c>
       <c r="F10" t="n">
+        <v>3</v>
+      </c>
+      <c r="G10" t="n">
         <v>2</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
+        <v>1680</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
         <v>1</v>
       </c>
-      <c r="H10" t="n">
-        <v>970</v>
-      </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" t="b">
-        <v>0</v>
-      </c>
       <c r="K10" t="b">
         <v>0</v>
       </c>
@@ -1342,87 +1344,83 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>1920</v>
+        <v>2004</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/181-E-Lewelling-Blvd-94580/home/1021451</t>
+          <t>https://www.redfin.com/CA/Ashland/934-Delano-St-94580/home/1255041</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Open House - 1:00 - 4:00 PM</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Apr 13, 1:00PM</t>
         </is>
       </c>
       <c r="Q10" t="n">
-        <v>3849880374</v>
+        <v>2635553646</v>
       </c>
       <c r="R10" t="n">
         <v>0</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>Kathi Townsend</t>
+          <t>Harry Cordiano</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>ATTENTION DEVELOPERS! THIS PROPERTY BOASTS ENDLESS POSSIBILITIES. Two lots equaling 1 Acre. Check with County to see how many units can be built on property. Possible uses include a family compound or possibly multiple families, business use to park or store multiple vehicles, i. e. , Landscapers can have equipment and plants and family all on one property. You can build ADU's and have family and income. Main house has 2 bedrooms, 1 bath, and is 970 sq. ft. Property also as a detached garage and 2 storage structures. Property to be sold in conjunction with adjoining lot at 183 E Lewelling Blvd.</t>
+          <t>Come check out this amazing single-family home that offers 3 bedrooms and 2 bathrooms, providing 1,680 square feet of living space in a single story floor plan, with easy daily functionality, and abundant natural light from multiple skylights throughout. Separate formal living, and formal dining areas with raised ceilings, an oversized eat-in kitchen with lots of storage and walk-in pantry. You’ll love the primary bedroom suite with access to backyard area, and primary bathroom with shower enclosure, jetted sunken tub and walk-in closet. Gorgeous backyard area with wooden deck and mature avocado tree. Out front an impressive 483 sqft detached two-car garage (21' by 23') with workbench</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>ASHLAND</t>
+          <t>ASHLAND UNINCORP</t>
         </is>
       </c>
       <c r="V10" t="n">
-        <v>37.6864694</v>
+        <v>37.6928735</v>
       </c>
       <c r="W10" t="n">
-        <v>-122.1194013</v>
+        <v>-122.1164729</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>41048418</t>
+          <t>ML81997607</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21266 Garden Ave</t>
+          <t>467 Albion Ave</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Hayward</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>94541</t>
+          <t>94580</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2299000</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>No beds info</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>No baths info</t>
-        </is>
+        <v>1450000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9</v>
       </c>
       <c r="H11" t="n">
-        <v>4788</v>
+        <v>3749</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -1439,11 +1437,11 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>1960</v>
+        <v>1952</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/Hayward/21266-Garden-Ave-94541/home/1285718</t>
+          <t>https://www.redfin.com/CA/Ashland/467-Albion-Ave-94580/home/1348996</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1457,7 +1455,7 @@
         </is>
       </c>
       <c r="Q11" t="n">
-        <v>3857804380</v>
+        <v>2710334593</v>
       </c>
       <c r="R11" t="inlineStr">
         <is>
@@ -1466,58 +1464,58 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>Satish Datt</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>FIVE UNIT MIXED PROPERTY: 20,380 sq ft lot with approximately 4,788 sq ft of living space. Single family homes with 2 bedrooms and 1.5 baths and 3 bedrooms and 2 baths. Triplex building with Three- 2 bedrooms and 1.5 baths each. Spacious floorplans. Each unit has 2 parking spaces and garages. Most of the units have some upgrades. Great location! Convenient to commute routes-880 freeway, and BART (Hayward station is close by). Property is close to 3 Colleges: Cal State East Bay. Chabot College and Mills college. Oakland airport is close by and easy access to the Peninsula.</t>
+          <t xml:space="preserve">Excellent price per unit and strong returns on day 1 with exceptional upside. The Azucena Group presents 467 Albion Ave. , a nine-unit multifamily property in San Lorenzo, featuring a unit mix of five studios and four one-bedroom, one-bathroom apartments. Situated on a large 0.29-acre lot (12,415 sq. ft. ), the property offers residents convenient amenities, including on-site parking and laundry facilities. Its prime location provides walkable access to numerous shops and services. Additionally, the property presents multiple value-add opportunities, allowing investors to enhance cash flow and increase asset value while investing in a community that connects the East Bay with the Peninsula </t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>Hayward</t>
+          <t>SAN LORENZO</t>
         </is>
       </c>
       <c r="V11" t="n">
-        <v>37.6683457</v>
+        <v>37.6859184</v>
       </c>
       <c r="W11" t="n">
-        <v>-122.1110595</v>
+        <v>-122.1292065</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>41045837</t>
+          <t>41088691</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21132 Garden Ave</t>
+          <t>16085 Via Pinal</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Hayward</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>94541</t>
+          <t>94580</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1100000</v>
+        <v>890000</v>
       </c>
       <c r="F12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G12" t="n">
         <v>2</v>
       </c>
       <c r="H12" t="n">
-        <v>2355</v>
+        <v>1765</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -1534,11 +1532,11 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>1938</v>
+        <v>1944</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/Hayward/21132-Garden-Ave-94541/home/1258762</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/16085-Via-Pinale-94580/home/1152482</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
@@ -1552,69 +1550,65 @@
         </is>
       </c>
       <c r="Q12" t="n">
-        <v>7728532617</v>
+        <v>3120155937</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>Meng Wu Moser</t>
+          <t>Zheng He</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>Great opportunity for you to add on to this 3 bed 2 bath house on the 13,000 lot. Huge backyard that is currently a working orchard and the house has a water producing well. 21164 Garden Ave is also for sale. Two lots together could be a new site for multiple-unit development; please confirm with Alameda County. Convenient central location in the Bay Area and just a few minutes to Highway 880 and Highway 92 to the Peninsula.</t>
+          <t>This beautifully updated home in the heart of San Lorenzo Village offers 4 bedrooms, 2 bathrooms, and 1,765 sq. ft. of comfortable living space. Step inside to a bright and inviting entryway that opens to a cozy living room, complete with a wood-burning fireplace—perfect for relaxing evenings. The open-concept layout seamlessly connects the living area to an updated kitchen featuring granite countertops, ample cabinet space, and a spacious dining area, overlooking the family room. Retreat to the spacious master suite, thoughtfully set apart from the main living areas for added privacy. It boasts a large closet, an updated en-suite bathroom, and private sliding door access to the seren</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>HAYWARD</t>
+          <t>SAN LORENZO VILG</t>
         </is>
       </c>
       <c r="V12" t="n">
-        <v>37.669084</v>
+        <v>37.6760155</v>
       </c>
       <c r="W12" t="n">
-        <v>-122.1114578</v>
+        <v>-122.1320642</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>41045472</t>
+          <t>41088418</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>20161 Royal Ave</t>
+          <t>1080 Via Palma</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Hayward</t>
+          <t>San Lorenzo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>94541</t>
+          <t>94580</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4280000</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>No beds info</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>No baths info</t>
-        </is>
+        <v>697000</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>10031</v>
+        <v>916</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
@@ -1625,17 +1619,15 @@
       <c r="K13" t="b">
         <v>0</v>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>No HOA fee</t>
-        </is>
+      <c r="L13" t="n">
+        <v>13</v>
       </c>
       <c r="M13" t="n">
-        <v>2009</v>
+        <v>1949</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>https://www.redfin.com/CA/Hayward/20161-Royal-Ave-94541/home/797383</t>
+          <t>https://www.redfin.com/CA/San-Lorenzo/1080-Via-Palma-94580/home/940128</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -1649,44 +1641,42 @@
         </is>
       </c>
       <c r="Q13" t="n">
-        <v>8278837047</v>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+        <v>3220478490</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>Jun H. Lin</t>
+          <t>Kyle-keizi Borton</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>Discover this special gated multifamily property boasting 7 units 3-bedroom, 2-bath townhouse-style homes along with a bonus manager's Studio nestled at 20161-20173 Royal Ave, in the thriving San Lorenzo/Hayward, CA area. Constructed in 2009, this property spans a generous Lot Size of 20,328 Sq ft (0.47 Acres), offering a gross living space of approximately 10,031 Sq ft. , designed with Subdivision Plan excellence and potential for subdivision. Each unit, meticulously designed, spans from approximately 1,269 SF to 1,794 SF, providing ample living space. Additionally, the manager's Studio offers around 600 SF. Ensuring convenience, every unit includes a two-car garage, providing a total of 1</t>
+          <t xml:space="preserve">FIXER   FIXER   FIXER  *  * Charming San Lorenzo Home! *  *  Welcome to 1080 Via Palma—a delightful single-family home featuring  *  * 2 bedrooms *  *  and  *  * 1 bathroom *  * . This cozy residence offers  *  * 916 sq ft *  *  of living space, perfect for first-time homebuyers or those looking to downsize. The home boasts a  *  * spacious living room with a fireplace *  * , and a comfortable dining area. The property sits on a  *  * 5,610 sq ft lot *  * , providing ample outdoor space for gardening, entertaining, or simply relaxing. Located in a friendly neighborhood, this home is close to  *  * schools, parks, shopping centers, and public transportation *  * . Enjoy easy access to </t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>Hayward</t>
+          <t>LORENZO VILLAGE</t>
         </is>
       </c>
       <c r="V13" t="n">
-        <v>37.6691682</v>
+        <v>37.6689226</v>
       </c>
       <c r="W13" t="n">
-        <v>-122.1159182</v>
+        <v>-122.1301987</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>41045725</t>
+          <t>41087652</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16066 Silverleaf Dr</t>
+          <t>17800 Via Toledo</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1700,73 +1690,738 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>964000</v>
+        <v>898800</v>
       </c>
       <c r="F14" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1353</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>13</v>
+      </c>
+      <c r="M14" t="n">
+        <v>1951</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/San-Lorenzo/17800-Via-Toledo-94580/home/1723499</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Open House - 1:00 - 4:00 PM</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>Apr 13, 1:00PM</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>3469030239</v>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>David Wilhite</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Great Value! Compare Recent Sales. Financing Terms: FHA, VA, Conventional Loans lower cash down payments. BRAND NEW ROOF! Affordable Sharp, Clean 3+ Bedroom 2 Bath ranch style house in San Lorenzo Village. House is located near community park. Nice curb appeal. Freshly painted inside. New flooring and carpet in many rooms. New draperies. Family room could become a 4th bedroom and make a primary suite with primary bath. 2nd Bath has tub with jets, dual sink basin custom mirrors and circular stain glass window. Formal dining area, updated bathrooms, central kitchen has built in gas range, double ovens, many updated cabinets with new hardware. MOVE-IN CONDITION! Property is nicely landscaped a</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>SAN LORENZO VILG</t>
+        </is>
+      </c>
+      <c r="V14" t="n">
+        <v>37.6791349</v>
+      </c>
+      <c r="W14" t="n">
+        <v>-122.1178483</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>41082065</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>20363 Royal Ave</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hayward</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>94541</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>661888</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1221</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>380</v>
+      </c>
+      <c r="M15" t="n">
+        <v>2004</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/Hayward-Acres/20363-Royal-Ave-94541/home/2115300</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>6408627780</v>
+      </c>
+      <c r="R15" t="n">
+        <v>1</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Zeke Mujaddadi</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Commuter’s Paradise in Alameda County!  Perfectly positioned midway along Hwy 880 with seamless connections to Hwy 238 and the San Mateo 92 Bridge, this end-unit townhouse is an ideal choice for those on the go. Enjoy quick access to Home Depot, supermarkets, diverse restaurants, and the relaxing Kennedy Park. Downtown Hayward's vibrant energy and the BART station are just a short drive away. Tucked in a quiet corner of a gated community, this well-maintained townhouse boasts a sunny and thoughtful layout. The home features two master suites, each with its own full bathroom, plus a convenient guest bath on the ground level. The open-concept living and dining areas are perfect for ente</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>CENTRAL HAYWARD</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
+        <v>37.668875</v>
+      </c>
+      <c r="W15" t="n">
+        <v>-122.1157502</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>41083108</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>920 Elgin St Unit G</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>94580</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>448000</v>
+      </c>
+      <c r="F16" t="n">
+        <v>2</v>
+      </c>
+      <c r="G16" t="n">
+        <v>2</v>
+      </c>
+      <c r="H16" t="n">
+        <v>900</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" t="n">
+        <v>450</v>
+      </c>
+      <c r="M16" t="n">
+        <v>1990</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/Ashland/920-Elgin-St-94580/unit-G/home/1810369</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>6948750838</v>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Karen Ostil</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Welcome to this cozy and affordable home, nestled in a secure gated complex on a quiet street. Conveniently located near local freeways and within walking distance to the BART station, this home offers the perfect mix of tranquility and accessibility. Inside this second-level unit, you’ll find an open floor plan with laminate and tile flooring, creating a practical and inviting living space. The kitchen features tile countertops, ample cabinet storage, and a functional layout perfect for meal preparation. A sliding glass door fills the space with natural light and leads to a charming patio—great for relaxing, adding greenery, or accessing the extra storage closet. The unit inclu</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>ASHLAND</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
+        <v>37.6914613</v>
+      </c>
+      <c r="W16" t="n">
+        <v>-122.1164255</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>PW25014911</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1773 Keller Ave</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>94580</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1870</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>No HOA fee</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>1952</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/San-Lorenzo/1773-Keller-Ave-94580/home/1071425</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>7024052021</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Investment - Investment!!!!    Beautiful House with RARE ADU (Second Unit) behind it!! This is like buying a duplex or 2 on 1 in a residential area. Approximately 1 mile from San Francisco Bay. Front House is a 3 Bedroom 1 3/4 Bathroom Remodeled Kitchen, (Just shy of 1200 sq-ft). The RARE ADU is a 2 Bedroom 1 Bathroom (Just shy of 700 sq-ft). This ADU is a Dream come True. There are not many of these ADU's around. This is set up for extra large Family. Kids or parents that are now living with you and you NEED the added Space. The Rear yard is also beautiful and very, very spacious. You could entertain the entire extended family and friends in such a wonderful and magnificent setting    1870</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="V17" t="n">
+        <v>37.6692606</v>
+      </c>
+      <c r="W17" t="n">
+        <v>-122.1416657</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>41082096</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>181 E Lewelling Blvd</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>94580</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1100000</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" t="n">
+        <v>970</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>No HOA fee</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>1920</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/Ashland/181-E-Lewelling-Blvd-94580/home/1021451</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>7972458116</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Kathi Townsend</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Cute cottage located on a 1/2 acre lot offering 2-bedrooms, 1-bath, laundry room screened-in patio and walk-in tool shed. Kitchen and bathroom have been updated.</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>ASHLAND</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
+        <v>37.6864855</v>
+      </c>
+      <c r="W18" t="n">
+        <v>-122.1194141</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>41082097</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>183 E Lewelling Blvd</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>94580</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>1300000</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" t="n">
         <v>4</v>
       </c>
-      <c r="G14" t="n">
-        <v>3</v>
-      </c>
-      <c r="H14" t="n">
-        <v>1948</v>
-      </c>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" t="b">
-        <v>0</v>
-      </c>
-      <c r="K14" t="b">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>116</v>
-      </c>
-      <c r="M14" t="n">
-        <v>1997</v>
-      </c>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>https://www.redfin.com/CA/San-Lorenzo/16066-Silverleaf-Dr-94580/home/797928</t>
-        </is>
-      </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="Q14" t="n">
-        <v>7999488364</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>Percy Cheung</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>Seller may carry 2nd loan. 4 bedroom and 3 full baths single family home with 1 bedroom, full bath on ground level. High ceiling in living room. Interior freshly painted. Mostly new engineer wood. flooring. End of court location with additional 3 car off street parking plus double car garage. Spacious rear yard.</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>MONTARA</t>
-        </is>
-      </c>
-      <c r="V14" t="n">
-        <v>37.6970246</v>
-      </c>
-      <c r="W14" t="n">
-        <v>-122.1194456</v>
+      <c r="H19" t="n">
+        <v>2648</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>No HOA fee</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>1920</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/Ashland/183-E-Lewelling-Blvd-94580/home/1847919</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>7972957907</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Kathi Townsend</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Situated on a 1/2 acre lot, this property consists of a Craftsman style house with 2 bedrooms, den, laundry room, partial basement plus an updated kitchen and bathroom. Also located on the property are three (3) detached studio or 1 bedroom, 1 bathroom rental cottages.</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="V19" t="n">
+        <v>37.6864823</v>
+      </c>
+      <c r="W19" t="n">
+        <v>-122.1190638</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>41079969</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>15540 Hesperian Blvd</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>94580</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>1080000</v>
+      </c>
+      <c r="F20" t="n">
+        <v>5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1564</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>No HOA fee</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>1910</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/Ashland/15540-Hesperian-Blvd-94580/home/1969205</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q20" t="n">
+        <v>11088259824</v>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Wilson Ou</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Great Commercial Investments. Prime location -Two parcels zoned as commercial. One parcel has a 3 bedroom 1 bath SFR house in front and rear Duplex with two 1 bd 1 bath units. Another parcel has 7 rooms 2 bath office/retail, currently using as Kitchen  &amp;  Bathroom showroom  &amp;  Storage. Adjoining to a shopping strip and across the street from Walmart. Potential to add more retail/office units. (check with Alameda county zoning/planning office. Current zoning - District Commercial - allows to build up to 5 stories, 75' high building for conditional use permit. Zoned for studio, art, dance, martial arts, music, theater, cinema of performing art, library, museum, art gallery, office, me</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>37.6882588</v>
+      </c>
+      <c r="W20" t="n">
+        <v>-122.1297389</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>41059501</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0 E 14th St</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>94580</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>300000</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>No beds info</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>No baths info</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>4500</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>No HOA fee</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>Year built not provided</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>https://www.redfin.com/CA/San-Leandro/E-14th-St-Unknown/home/147101770</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="Q21" t="n">
+        <v>28905969412</v>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Cristina Kaady</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Centrally located Commercial Lot for Sale! This lot is near shopping, dining, hospitals, Cinemas and Transportation. Across the street from Bayfair Shopping Center!  Nestled between 580, 880 and 238 Freeways for easy access! Great visibility for what you decide to build or operate. Check the County for all your possibilities! The Lot fronts east 14th Street located between 15772 and 15796 East 14Th Street.</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>San Lorenzo</t>
+        </is>
+      </c>
+      <c r="V21" t="n">
+        <v>37.6803</v>
+      </c>
+      <c r="W21" t="n">
+        <v>-122.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>